<commit_message>
dropdown working left, need to push now and start a new fresh day coding
</commit_message>
<xml_diff>
--- a/Excel/inventory.xlsx
+++ b/Excel/inventory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>Category</t>
   </si>
@@ -40,6 +40,9 @@
     <t>Condition</t>
   </si>
   <si>
+    <t>Owning_Date</t>
+  </si>
+  <si>
     <t>Electronics</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>Name9</t>
   </si>
   <si>
+    <t>as</t>
+  </si>
+  <si>
     <t>Make1</t>
   </si>
   <si>
@@ -103,6 +109,9 @@
     <t>Make9</t>
   </si>
   <si>
+    <t>asd</t>
+  </si>
+  <si>
     <t>Model1</t>
   </si>
   <si>
@@ -130,6 +139,9 @@
     <t>Model9</t>
   </si>
   <si>
+    <t>sd</t>
+  </si>
+  <si>
     <t>Serial1</t>
   </si>
   <si>
@@ -157,6 +169,9 @@
     <t>Serial9</t>
   </si>
   <si>
+    <t>ss</t>
+  </si>
+  <si>
     <t>SOI ASSAM</t>
   </si>
   <si>
@@ -187,7 +202,10 @@
     <t>Damaged</t>
   </si>
   <si>
-    <t>aaa</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Good</t>
   </si>
 </sst>
 </file>
@@ -545,13 +563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,239 +594,268 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="E11" t="s">
         <v>51</v>
       </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F11" t="s">
         <v>52</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" t="s">
-        <v>53</v>
+      <c r="H11" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel Updated, Stage Errorssss, Logout Solved,  Transaction Status Tafseer.
</commit_message>
<xml_diff>
--- a/Excel/inventory.xlsx
+++ b/Excel/inventory.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\shazli\Inventory-Management-System\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
   <si>
     <t>Category</t>
   </si>
@@ -79,9 +84,6 @@
     <t>Name9</t>
   </si>
   <si>
-    <t>as</t>
-  </si>
-  <si>
     <t>Make1</t>
   </si>
   <si>
@@ -109,9 +111,6 @@
     <t>Make9</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
     <t>Model1</t>
   </si>
   <si>
@@ -139,9 +138,6 @@
     <t>Model9</t>
   </si>
   <si>
-    <t>sd</t>
-  </si>
-  <si>
     <t>Serial1</t>
   </si>
   <si>
@@ -169,7 +165,22 @@
     <t>Serial9</t>
   </si>
   <si>
-    <t>ss</t>
+    <t>Serial12</t>
+  </si>
+  <si>
+    <t>Serial13</t>
+  </si>
+  <si>
+    <t>Serial14</t>
+  </si>
+  <si>
+    <t>Serial15</t>
+  </si>
+  <si>
+    <t>Serial16</t>
+  </si>
+  <si>
+    <t>Serial17</t>
   </si>
   <si>
     <t>SOI TRIPURA</t>
@@ -178,44 +189,92 @@
     <t>SOI ASSAM</t>
   </si>
   <si>
-    <t>Fahad</t>
-  </si>
-  <si>
-    <t>Zafar</t>
-  </si>
-  <si>
-    <t>Umar</t>
-  </si>
-  <si>
-    <t>Hammad</t>
-  </si>
-  <si>
-    <t>badhiya</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>Nan</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Damaged</t>
-  </si>
-  <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>EA2</t>
+  </si>
+  <si>
+    <t>MJ2</t>
+  </si>
+  <si>
+    <t>MO1</t>
+  </si>
+  <si>
+    <t>ES1</t>
+  </si>
+  <si>
+    <t>Name10</t>
+  </si>
+  <si>
+    <t>Name11</t>
+  </si>
+  <si>
+    <t>Name12</t>
+  </si>
+  <si>
+    <t>Name13</t>
+  </si>
+  <si>
+    <t>Name14</t>
+  </si>
+  <si>
+    <t>Name15</t>
+  </si>
+  <si>
+    <t>Make10</t>
+  </si>
+  <si>
+    <t>Make11</t>
+  </si>
+  <si>
+    <t>Make12</t>
+  </si>
+  <si>
+    <t>Make13</t>
+  </si>
+  <si>
+    <t>Make14</t>
+  </si>
+  <si>
+    <t>Make15</t>
+  </si>
+  <si>
+    <t>Model10</t>
+  </si>
+  <si>
+    <t>Model11</t>
+  </si>
+  <si>
+    <t>Model12</t>
+  </si>
+  <si>
+    <t>Model13</t>
+  </si>
+  <si>
+    <t>Model14</t>
+  </si>
+  <si>
+    <t>Model15</t>
+  </si>
+  <si>
+    <t>Name16</t>
+  </si>
+  <si>
+    <t>Make16</t>
+  </si>
+  <si>
+    <t>Model16</t>
+  </si>
+  <si>
+    <t>Serial18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +337,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -324,7 +391,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,9 +423,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,6 +458,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -565,14 +634,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -609,25 +686,25 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -635,25 +712,25 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -661,25 +738,25 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -687,25 +764,25 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -713,25 +790,25 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -739,25 +816,25 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -765,25 +842,25 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -791,25 +868,25 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
         <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -817,48 +894,204 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" t="s">
         <v>52</v>
       </c>
-      <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="G11" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" t="s">
-        <v>64</v>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>